<commit_message>
Update Database có thể sẽ lỗi
</commit_message>
<xml_diff>
--- a/KoiManagement/Content/FileImport/Koi.xlsx
+++ b/KoiManagement/Content/FileImport/Koi.xlsx
@@ -39,26 +39,165 @@
     <t>Ảnh 5</t>
   </si>
   <si>
-    <t>Tên cá koi(*)</t>
-  </si>
-  <si>
-    <t>Ngày sinh(dd/MM/YYYY)</t>
-  </si>
-  <si>
-    <t>Kích thước(cm)(*)</t>
-  </si>
-  <si>
-    <t>Ảnh 1(Ảnh đại diện)(*)</t>
+    <r>
+      <t>Tên cá koi(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ngày sinh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(dd/MM/YYYY)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Kích thước</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(cm)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ảnh 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Ảnh đại diện)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -391,7 +530,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,9 +584,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D2" s="1">
-        <v>33209</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -459,6 +596,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>